<commit_message>
Map Toolkit SQL Server resource utilization
</commit_message>
<xml_diff>
--- a/Excel Sheets/Map Toolkit SQL Server resource utilization report Template.xlsx
+++ b/Excel Sheets/Map Toolkit SQL Server resource utilization report Template.xlsx
@@ -36,7 +36,7 @@
   </definedNames>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="4" r:id="rId15"/>
+    <pivotCache cacheId="0" r:id="rId15"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="134">
   <si>
     <t>CPU</t>
   </si>
@@ -480,6 +480,12 @@
   <si>
     <t>Status</t>
   </si>
+  <si>
+    <t>SQL Services Running</t>
+  </si>
+  <si>
+    <t>SQL Services Stopped</t>
+  </si>
 </sst>
 </file>
 
@@ -611,7 +617,7 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -709,13 +715,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Farve1" xfId="2" builtinId="29"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Procent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="128">
+  <dxfs count="132">
     <dxf>
       <font>
         <b val="0"/>
@@ -836,6 +845,54 @@
         </patternFill>
       </fill>
       <alignment horizontal="right" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -2016,7 +2073,7 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
+        <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -2031,11 +2088,16 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
-        <b/>
+        <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -2050,60 +2112,12 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -2241,6 +2255,82 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -2318,13 +2408,28 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="right" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -10984,6 +11089,168 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
+      <xdr:colOff>161924</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>333375</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>952499</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>666750</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="Tekstboks 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1936E260-3319-4583-8AC1-DE6A452ACCC7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="161924" y="333375"/>
+          <a:ext cx="9658350" cy="333375"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="da-DK" sz="1800" b="1"/>
+            <a:t>SQL Virtual pltaform hardware </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="da-DK" sz="1800" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>details</a:t>
+          </a:r>
+          <a:endParaRPr lang="da-DK" sz="1800"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="da-DK" sz="1800" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>382141</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Billede 6" descr="Image result for solidq">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A4584341-A520-43C4-9036-66D44B7DC683}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="1266825" cy="382141"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
       <xdr:colOff>180974</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>352425</xdr:rowOff>
@@ -11134,7 +11401,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -11300,7 +11567,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -11344,7 +11611,7 @@
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Raoul" refreshedDate="42870.576583333335" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="62">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A1:AA1048576" sheet="Consolidation overview - Runnin"/>
+    <worksheetSource ref="A1:AC1048576" sheet="Consolidation overview - Runnin"/>
   </cacheSource>
   <cacheFields count="27">
     <cacheField name="Computer Name" numFmtId="0">
@@ -13251,7 +13518,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Pivottabel6" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Værdier" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Pivottabel6" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Værdier" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
   <location ref="A3:B5" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="27">
     <pivotField dataField="1" subtotalTop="0" showAll="0"/>
@@ -13374,7 +13641,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Pivottabel1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Værdier" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="5">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Pivottabel1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Værdier" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="5">
   <location ref="A3:B4" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="27">
     <pivotField subtotalTop="0" showAll="0"/>
@@ -13461,7 +13728,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Pivottabel3" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Værdier" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="6">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Pivottabel3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Værdier" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="6">
   <location ref="A1:B2" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="27">
     <pivotField subtotalTop="0" showAll="0"/>
@@ -13548,7 +13815,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Pivottabel4" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Værdier" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Pivottabel4" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Værdier" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
   <location ref="A1:C2" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="27">
     <pivotField subtotalTop="0" showAll="0"/>
@@ -13827,9 +14094,9 @@
   <autoFilter ref="A19:D22"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Calculations"/>
-    <tableColumn id="4" name="Percentage" dataDxfId="127"/>
-    <tableColumn id="2" name="CPUs" dataDxfId="126"/>
-    <tableColumn id="3" name="Cores" dataDxfId="125"/>
+    <tableColumn id="4" name="Percentage" dataDxfId="131"/>
+    <tableColumn id="2" name="CPUs" dataDxfId="130"/>
+    <tableColumn id="3" name="Cores" dataDxfId="129"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -13847,110 +14114,112 @@
     <tableColumn id="35" uniqueName="35" name="Operated By" queryTableFieldId="54"/>
     <tableColumn id="34" uniqueName="34" name="Environment" queryTableFieldId="53"/>
     <tableColumn id="2" uniqueName="2" name="Operating System" queryTableFieldId="2"/>
-    <tableColumn id="6" uniqueName="6" name="CPU" queryTableFieldId="6" dataDxfId="107"/>
-    <tableColumn id="7" uniqueName="7" name="CPU Speed (GHz)" queryTableFieldId="7" dataDxfId="106"/>
-    <tableColumn id="55" uniqueName="55" name="Number of Processors" queryTableFieldId="57" dataDxfId="105"/>
-    <tableColumn id="54" uniqueName="54" name="Number of Cores" queryTableFieldId="56" dataDxfId="104"/>
-    <tableColumn id="8" uniqueName="8" name="Logical Processor Count" queryTableFieldId="8" dataDxfId="103"/>
-    <tableColumn id="9" uniqueName="9" name="Average CPU Utilization (%)" queryTableFieldId="9" dataDxfId="102"/>
-    <tableColumn id="10" uniqueName="10" name="Maximum CPU Utilization (%)" queryTableFieldId="10" dataDxfId="101"/>
-    <tableColumn id="11" uniqueName="11" name="95th Percentile CPU Utilization (%)" queryTableFieldId="11" dataDxfId="100"/>
-    <tableColumn id="12" uniqueName="12" name="Memory (MB)" queryTableFieldId="12" dataDxfId="99"/>
-    <tableColumn id="13" uniqueName="13" name="Average Memory Utilization (GB)" queryTableFieldId="13" dataDxfId="98"/>
-    <tableColumn id="14" uniqueName="14" name="Maximum Memory Utilization (GB)" queryTableFieldId="14" dataDxfId="97"/>
-    <tableColumn id="15" uniqueName="15" name="95th Percentile Memory Utilization (GB)" queryTableFieldId="15" dataDxfId="96"/>
-    <tableColumn id="16" uniqueName="16" name="Average Disk IOPS" queryTableFieldId="16" dataDxfId="95"/>
-    <tableColumn id="17" uniqueName="17" name="Maximum Disk IOPS" queryTableFieldId="17" dataDxfId="94"/>
-    <tableColumn id="18" uniqueName="18" name="95th Percentile Disk IOPS" queryTableFieldId="18" dataDxfId="93"/>
-    <tableColumn id="19" uniqueName="19" name="Avg Disk Writes/sec" queryTableFieldId="19" dataDxfId="92"/>
-    <tableColumn id="20" uniqueName="20" name="Max Disk Writes/sec" queryTableFieldId="20" dataDxfId="91"/>
-    <tableColumn id="21" uniqueName="21" name="95th Percentile Disk Writes/sec" queryTableFieldId="21" dataDxfId="90"/>
-    <tableColumn id="22" uniqueName="22" name="Avg Disk Reads/sec" queryTableFieldId="22" dataDxfId="89"/>
-    <tableColumn id="23" uniqueName="23" name="Max Disk Reads/sec" queryTableFieldId="23" dataDxfId="88"/>
-    <tableColumn id="24" uniqueName="24" name="95th Percentile Disk Reads/sec" queryTableFieldId="24" dataDxfId="87"/>
-    <tableColumn id="25" uniqueName="25" name="Average Network Utilization (MB/s)" queryTableFieldId="25" dataDxfId="86"/>
-    <tableColumn id="26" uniqueName="26" name="Maximum Network Utilization (MB/s)" queryTableFieldId="26" dataDxfId="85"/>
-    <tableColumn id="27" uniqueName="27" name="95th Percentile Network Utilization (MB/s)" queryTableFieldId="27" dataDxfId="84"/>
-    <tableColumn id="28" uniqueName="28" name="Avg Network Bytes Sent (MB/s)" queryTableFieldId="28" dataDxfId="83"/>
-    <tableColumn id="29" uniqueName="29" name="Max Network Bytes Sent (MB/s)" queryTableFieldId="29" dataDxfId="82"/>
-    <tableColumn id="30" uniqueName="30" name="95th Percentile Network Bytes Sent (MB/s)" queryTableFieldId="30" dataDxfId="81"/>
-    <tableColumn id="31" uniqueName="31" name="Avg Network Bytes Received (MB/s)" queryTableFieldId="31" dataDxfId="80"/>
-    <tableColumn id="32" uniqueName="32" name="Max Network Bytes Received (MB/s)" queryTableFieldId="32" dataDxfId="79"/>
-    <tableColumn id="33" uniqueName="33" name="95th Percentile Network Bytes Received (MB/s)" queryTableFieldId="33" dataDxfId="78"/>
-    <tableColumn id="36" uniqueName="36" name="Average Disk Space Utilization (GB)" queryTableFieldId="36" dataDxfId="77"/>
-    <tableColumn id="37" uniqueName="37" name="Maximum Disk Space Utilization (GB)" queryTableFieldId="37" dataDxfId="76"/>
-    <tableColumn id="38" uniqueName="38" name="95th Percentile Disk Space Utilization (GB)" queryTableFieldId="38" dataDxfId="75"/>
-    <tableColumn id="39" uniqueName="39" name="Avg Disk Queue Length" queryTableFieldId="39" dataDxfId="74"/>
-    <tableColumn id="40" uniqueName="40" name="Max Disk Queue Length" queryTableFieldId="40" dataDxfId="73"/>
-    <tableColumn id="41" uniqueName="41" name="95th Percentile Disk Queue Length" queryTableFieldId="41" dataDxfId="72"/>
-    <tableColumn id="42" uniqueName="42" name="Avg Disk Read Queue Length" queryTableFieldId="42" dataDxfId="71"/>
-    <tableColumn id="43" uniqueName="43" name="Max Disk Read Queue Length" queryTableFieldId="43" dataDxfId="70"/>
-    <tableColumn id="44" uniqueName="44" name="95th Percentile Disk Read Queue Length" queryTableFieldId="44" dataDxfId="69"/>
-    <tableColumn id="45" uniqueName="45" name="Avg Disk Write Queue Length" queryTableFieldId="45" dataDxfId="68"/>
-    <tableColumn id="46" uniqueName="46" name="Max Disk Write Queue Length" queryTableFieldId="46" dataDxfId="67"/>
-    <tableColumn id="47" uniqueName="47" name="95th Percentile Disk Write Queue Length" queryTableFieldId="47" dataDxfId="66"/>
-    <tableColumn id="48" uniqueName="48" name="Avg Disk Bytes/sec" queryTableFieldId="50" dataDxfId="65"/>
-    <tableColumn id="49" uniqueName="49" name="Max Disk Bytes/sec" queryTableFieldId="49" dataDxfId="64"/>
-    <tableColumn id="50" uniqueName="50" name="95th Percentile Disk Bytes/sec" queryTableFieldId="48" dataDxfId="63"/>
+    <tableColumn id="6" uniqueName="6" name="CPU" queryTableFieldId="6" dataDxfId="102"/>
+    <tableColumn id="7" uniqueName="7" name="CPU Speed (GHz)" queryTableFieldId="7" dataDxfId="101"/>
+    <tableColumn id="55" uniqueName="55" name="Number of Processors" queryTableFieldId="57" dataDxfId="100"/>
+    <tableColumn id="54" uniqueName="54" name="Number of Cores" queryTableFieldId="56" dataDxfId="99"/>
+    <tableColumn id="8" uniqueName="8" name="Logical Processor Count" queryTableFieldId="8" dataDxfId="98"/>
+    <tableColumn id="9" uniqueName="9" name="Average CPU Utilization (%)" queryTableFieldId="9" dataDxfId="97"/>
+    <tableColumn id="10" uniqueName="10" name="Maximum CPU Utilization (%)" queryTableFieldId="10" dataDxfId="96"/>
+    <tableColumn id="11" uniqueName="11" name="95th Percentile CPU Utilization (%)" queryTableFieldId="11" dataDxfId="95"/>
+    <tableColumn id="12" uniqueName="12" name="Memory (MB)" queryTableFieldId="12" dataDxfId="94"/>
+    <tableColumn id="13" uniqueName="13" name="Average Memory Utilization (GB)" queryTableFieldId="13" dataDxfId="93"/>
+    <tableColumn id="14" uniqueName="14" name="Maximum Memory Utilization (GB)" queryTableFieldId="14" dataDxfId="92"/>
+    <tableColumn id="15" uniqueName="15" name="95th Percentile Memory Utilization (GB)" queryTableFieldId="15" dataDxfId="91"/>
+    <tableColumn id="16" uniqueName="16" name="Average Disk IOPS" queryTableFieldId="16" dataDxfId="90"/>
+    <tableColumn id="17" uniqueName="17" name="Maximum Disk IOPS" queryTableFieldId="17" dataDxfId="89"/>
+    <tableColumn id="18" uniqueName="18" name="95th Percentile Disk IOPS" queryTableFieldId="18" dataDxfId="88"/>
+    <tableColumn id="19" uniqueName="19" name="Avg Disk Writes/sec" queryTableFieldId="19" dataDxfId="87"/>
+    <tableColumn id="20" uniqueName="20" name="Max Disk Writes/sec" queryTableFieldId="20" dataDxfId="86"/>
+    <tableColumn id="21" uniqueName="21" name="95th Percentile Disk Writes/sec" queryTableFieldId="21" dataDxfId="85"/>
+    <tableColumn id="22" uniqueName="22" name="Avg Disk Reads/sec" queryTableFieldId="22" dataDxfId="84"/>
+    <tableColumn id="23" uniqueName="23" name="Max Disk Reads/sec" queryTableFieldId="23" dataDxfId="83"/>
+    <tableColumn id="24" uniqueName="24" name="95th Percentile Disk Reads/sec" queryTableFieldId="24" dataDxfId="82"/>
+    <tableColumn id="25" uniqueName="25" name="Average Network Utilization (MB/s)" queryTableFieldId="25" dataDxfId="81"/>
+    <tableColumn id="26" uniqueName="26" name="Maximum Network Utilization (MB/s)" queryTableFieldId="26" dataDxfId="80"/>
+    <tableColumn id="27" uniqueName="27" name="95th Percentile Network Utilization (MB/s)" queryTableFieldId="27" dataDxfId="79"/>
+    <tableColumn id="28" uniqueName="28" name="Avg Network Bytes Sent (MB/s)" queryTableFieldId="28" dataDxfId="78"/>
+    <tableColumn id="29" uniqueName="29" name="Max Network Bytes Sent (MB/s)" queryTableFieldId="29" dataDxfId="77"/>
+    <tableColumn id="30" uniqueName="30" name="95th Percentile Network Bytes Sent (MB/s)" queryTableFieldId="30" dataDxfId="76"/>
+    <tableColumn id="31" uniqueName="31" name="Avg Network Bytes Received (MB/s)" queryTableFieldId="31" dataDxfId="75"/>
+    <tableColumn id="32" uniqueName="32" name="Max Network Bytes Received (MB/s)" queryTableFieldId="32" dataDxfId="74"/>
+    <tableColumn id="33" uniqueName="33" name="95th Percentile Network Bytes Received (MB/s)" queryTableFieldId="33" dataDxfId="73"/>
+    <tableColumn id="36" uniqueName="36" name="Average Disk Space Utilization (GB)" queryTableFieldId="36" dataDxfId="72"/>
+    <tableColumn id="37" uniqueName="37" name="Maximum Disk Space Utilization (GB)" queryTableFieldId="37" dataDxfId="71"/>
+    <tableColumn id="38" uniqueName="38" name="95th Percentile Disk Space Utilization (GB)" queryTableFieldId="38" dataDxfId="70"/>
+    <tableColumn id="39" uniqueName="39" name="Avg Disk Queue Length" queryTableFieldId="39" dataDxfId="69"/>
+    <tableColumn id="40" uniqueName="40" name="Max Disk Queue Length" queryTableFieldId="40" dataDxfId="68"/>
+    <tableColumn id="41" uniqueName="41" name="95th Percentile Disk Queue Length" queryTableFieldId="41" dataDxfId="67"/>
+    <tableColumn id="42" uniqueName="42" name="Avg Disk Read Queue Length" queryTableFieldId="42" dataDxfId="66"/>
+    <tableColumn id="43" uniqueName="43" name="Max Disk Read Queue Length" queryTableFieldId="43" dataDxfId="65"/>
+    <tableColumn id="44" uniqueName="44" name="95th Percentile Disk Read Queue Length" queryTableFieldId="44" dataDxfId="64"/>
+    <tableColumn id="45" uniqueName="45" name="Avg Disk Write Queue Length" queryTableFieldId="45" dataDxfId="63"/>
+    <tableColumn id="46" uniqueName="46" name="Max Disk Write Queue Length" queryTableFieldId="46" dataDxfId="62"/>
+    <tableColumn id="47" uniqueName="47" name="95th Percentile Disk Write Queue Length" queryTableFieldId="47" dataDxfId="61"/>
+    <tableColumn id="48" uniqueName="48" name="Avg Disk Bytes/sec" queryTableFieldId="50" dataDxfId="60"/>
+    <tableColumn id="49" uniqueName="49" name="Max Disk Bytes/sec" queryTableFieldId="49" dataDxfId="59"/>
+    <tableColumn id="50" uniqueName="50" name="95th Percentile Disk Bytes/sec" queryTableFieldId="48" dataDxfId="58"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabel6" displayName="Tabel6" ref="A1:AA3" insertRow="1" totalsRowCount="1" dataCellStyle="Normal">
-  <autoFilter ref="A1:AA2"/>
-  <tableColumns count="27">
-    <tableColumn id="1" name="Computer Name" totalsRowDxfId="53" dataCellStyle="Normal"/>
-    <tableColumn id="2" name="Machine Type" totalsRowDxfId="52" dataCellStyle="Normal"/>
-    <tableColumn id="3" name="Operated By" totalsRowDxfId="51" dataCellStyle="Normal"/>
-    <tableColumn id="4" name="Environment" totalsRowDxfId="50" dataCellStyle="Normal"/>
-    <tableColumn id="5" name="System Model" totalsRowDxfId="49" dataCellStyle="Normal"/>
-    <tableColumn id="6" name="SiteName" totalsRowDxfId="48" dataCellStyle="Normal"/>
-    <tableColumn id="7" name="NumberOfClusteredInstances" totalsRowDxfId="47" dataCellStyle="Normal"/>
-    <tableColumn id="8" name="Current Operating System" totalsRowDxfId="46" dataCellStyle="Normal"/>
-    <tableColumn id="9" name="Operating System Architecture Type" totalsRowDxfId="45" dataCellStyle="Normal"/>
-    <tableColumn id="10" name="Number of SQL Instances" totalsRowFunction="custom" totalsRowDxfId="44" dataCellStyle="Normal">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabel6" displayName="Tabel6" ref="A1:AC3" insertRow="1" totalsRowCount="1" dataCellStyle="Normal">
+  <autoFilter ref="A1:AC2"/>
+  <tableColumns count="29">
+    <tableColumn id="1" name="Computer Name" totalsRowDxfId="57" dataCellStyle="Normal"/>
+    <tableColumn id="2" name="Machine Type" totalsRowDxfId="56" dataCellStyle="Normal"/>
+    <tableColumn id="3" name="Operated By" totalsRowDxfId="55" dataCellStyle="Normal"/>
+    <tableColumn id="4" name="Environment" totalsRowDxfId="54" dataCellStyle="Normal"/>
+    <tableColumn id="5" name="System Model" totalsRowDxfId="53" dataCellStyle="Normal"/>
+    <tableColumn id="6" name="SiteName" totalsRowDxfId="52" dataCellStyle="Normal"/>
+    <tableColumn id="7" name="NumberOfClusteredInstances" totalsRowDxfId="51" dataCellStyle="Normal"/>
+    <tableColumn id="8" name="Current Operating System" totalsRowDxfId="50" dataCellStyle="Normal"/>
+    <tableColumn id="9" name="Operating System Architecture Type" totalsRowDxfId="49" dataCellStyle="Normal"/>
+    <tableColumn id="10" name="Number of SQL Instances" totalsRowFunction="custom" totalsRowDxfId="48" dataCellStyle="Normal">
       <totalsRowFormula>SUM(J2:J2)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="11" name="Number Of Databases" totalsRowFunction="custom" totalsRowDxfId="43" dataCellStyle="Normal">
-      <totalsRowFormula>SUM(K2:K2)</totalsRowFormula>
-    </tableColumn>
-    <tableColumn id="12" name="Number of Processors" totalsRowFunction="custom" totalsRowDxfId="42" dataCellStyle="Normal">
-      <totalsRowFormula>SUM(L2:L2)</totalsRowFormula>
-    </tableColumn>
-    <tableColumn id="13" name="Number of Total Cores" totalsRowFunction="custom" totalsRowDxfId="41" dataCellStyle="Normal">
+    <tableColumn id="29" name="SQL Services Running" totalsRowDxfId="47"/>
+    <tableColumn id="27" name="SQL Services Stopped" totalsRowDxfId="46"/>
+    <tableColumn id="11" name="Number Of Databases" totalsRowFunction="custom" totalsRowDxfId="45" dataCellStyle="Normal">
       <totalsRowFormula>SUM(M2:M2)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="14" name="Number of Logical Processors" totalsRowFunction="custom" totalsRowDxfId="40" dataCellStyle="Normal">
+    <tableColumn id="12" name="Number of Processors" totalsRowFunction="custom" totalsRowDxfId="44" dataCellStyle="Normal">
       <totalsRowFormula>SUM(N2:N2)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="15" name="CPU" totalsRowDxfId="39" dataCellStyle="Normal"/>
-    <tableColumn id="16" name="System Memory (MB)" totalsRowDxfId="38" dataCellStyle="Normal"/>
-    <tableColumn id="17" name="System Memory (GB)" totalsRowFunction="custom" totalsRowDxfId="37" dataCellStyle="Normal">
-      <totalsRowFormula>SUM(Q2:Q2)</totalsRowFormula>
+    <tableColumn id="13" name="Number of Total Cores" totalsRowFunction="custom" totalsRowDxfId="43" dataCellStyle="Normal">
+      <totalsRowFormula>SUM(O2:O2)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="18" name="Logical Disk Size (GB)" totalsRowFunction="custom" totalsRowDxfId="36" dataCellStyle="Normal">
-      <totalsRowFormula>SUM(R2:R2)</totalsRowFormula>
+    <tableColumn id="14" name="Number of Logical Processors" totalsRowFunction="custom" totalsRowDxfId="42" dataCellStyle="Normal">
+      <totalsRowFormula>SUM(P2:P2)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="19" name="Logical Disk Free Space (GB)" totalsRowFunction="custom" totalsRowDxfId="35" dataCellStyle="Normal">
+    <tableColumn id="15" name="CPU" totalsRowDxfId="41" dataCellStyle="Normal"/>
+    <tableColumn id="16" name="System Memory (MB)" totalsRowDxfId="40" dataCellStyle="Normal"/>
+    <tableColumn id="17" name="System Memory (GB)" totalsRowFunction="custom" totalsRowDxfId="39" dataCellStyle="Normal">
       <totalsRowFormula>SUM(S2:S2)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="20" name="Logical Disk Size (TB)" totalsRowDxfId="34" dataCellStyle="Normal"/>
-    <tableColumn id="21" name="Logical Disk Free Space (TB)" totalsRowDxfId="33" dataCellStyle="Normal"/>
-    <tableColumn id="22" name="SuccessPercent" totalsRowDxfId="32" dataCellStyle="Normal"/>
-    <tableColumn id="28" name="Kolonne1" totalsRowLabel="Average:" totalsRowDxfId="31" dataCellStyle="Normal"/>
-    <tableColumn id="23" name="ProcUtil" totalsRowFunction="custom" totalsRowDxfId="30" dataCellStyle="Normal">
-      <totalsRowFormula>AVERAGE(X2:X2)</totalsRowFormula>
+    <tableColumn id="18" name="Logical Disk Size (GB)" totalsRowFunction="custom" totalsRowDxfId="38" dataCellStyle="Normal">
+      <totalsRowFormula>SUM(T2:T2)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="24" name="MemoryUtil" totalsRowFunction="custom" totalsRowDxfId="29" dataCellStyle="Normal">
-      <totalsRowFormula>AVERAGE(Y2:Y2)</totalsRowFormula>
+    <tableColumn id="19" name="Logical Disk Free Space (GB)" totalsRowFunction="custom" totalsRowDxfId="37" dataCellStyle="Normal">
+      <totalsRowFormula>SUM(U2:U2)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="25" name="NetworkUtil" totalsRowFunction="custom" totalsRowDxfId="28" dataCellStyle="Normal">
+    <tableColumn id="20" name="Logical Disk Size (TB)" totalsRowDxfId="36" dataCellStyle="Normal"/>
+    <tableColumn id="21" name="Logical Disk Free Space (TB)" totalsRowDxfId="35" dataCellStyle="Normal"/>
+    <tableColumn id="22" name="SuccessPercent" totalsRowDxfId="34" dataCellStyle="Normal"/>
+    <tableColumn id="28" name="Kolonne1" totalsRowLabel="Average:" totalsRowDxfId="33" dataCellStyle="Normal"/>
+    <tableColumn id="23" name="ProcUtil" totalsRowFunction="custom" totalsRowDxfId="32" dataCellStyle="Normal">
       <totalsRowFormula>AVERAGE(Z2:Z2)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="26" name="DiskIOPS" totalsRowFunction="custom" totalsRowDxfId="27" dataCellStyle="Normal">
+    <tableColumn id="24" name="MemoryUtil" totalsRowFunction="custom" totalsRowDxfId="31" dataCellStyle="Normal">
       <totalsRowFormula>AVERAGE(AA2:AA2)</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="25" name="NetworkUtil" totalsRowFunction="custom" totalsRowDxfId="30" dataCellStyle="Normal">
+      <totalsRowFormula>AVERAGE(AB2:AB2)</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="26" name="DiskIOPS" totalsRowFunction="custom" totalsRowDxfId="29" dataCellStyle="Normal">
+      <totalsRowFormula>AVERAGE(AC2:AC2)</totalsRowFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -13958,59 +14227,61 @@
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabel66" displayName="Tabel66" ref="A1:AA3" insertRow="1" totalsRowCount="1" dataCellStyle="Normal">
-  <autoFilter ref="A1:AA2"/>
-  <tableColumns count="27">
-    <tableColumn id="1" name="Computer Name" totalsRowDxfId="26" dataCellStyle="Normal"/>
-    <tableColumn id="2" name="Machine Type" totalsRowDxfId="25" dataCellStyle="Normal"/>
-    <tableColumn id="3" name="Operated By" totalsRowDxfId="24" dataCellStyle="Normal"/>
-    <tableColumn id="4" name="Environment" totalsRowDxfId="23" dataCellStyle="Normal"/>
-    <tableColumn id="5" name="System Model" totalsRowDxfId="22" dataCellStyle="Normal"/>
-    <tableColumn id="6" name="SiteName" totalsRowDxfId="21" dataCellStyle="Normal"/>
-    <tableColumn id="7" name="NumberOfClusteredInstances" totalsRowDxfId="20" dataCellStyle="Normal"/>
-    <tableColumn id="8" name="Current Operating System" totalsRowDxfId="19" dataCellStyle="Normal"/>
-    <tableColumn id="9" name="Operating System Architecture Type" totalsRowDxfId="18" dataCellStyle="Normal"/>
-    <tableColumn id="10" name="Number of SQL Instances" totalsRowFunction="custom" totalsRowDxfId="17" dataCellStyle="Normal">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabel66" displayName="Tabel66" ref="A1:AC3" insertRow="1" totalsRowCount="1" dataCellStyle="Normal">
+  <autoFilter ref="A1:AC2"/>
+  <tableColumns count="29">
+    <tableColumn id="1" name="Computer Name" totalsRowDxfId="28" dataCellStyle="Normal"/>
+    <tableColumn id="2" name="Machine Type" totalsRowDxfId="27" dataCellStyle="Normal"/>
+    <tableColumn id="3" name="Operated By" totalsRowDxfId="26" dataCellStyle="Normal"/>
+    <tableColumn id="4" name="Environment" totalsRowDxfId="25" dataCellStyle="Normal"/>
+    <tableColumn id="5" name="System Model" totalsRowDxfId="24" dataCellStyle="Normal"/>
+    <tableColumn id="6" name="SiteName" totalsRowDxfId="23" dataCellStyle="Normal"/>
+    <tableColumn id="7" name="NumberOfClusteredInstances" totalsRowDxfId="22" dataCellStyle="Normal"/>
+    <tableColumn id="8" name="Current Operating System" totalsRowDxfId="21" dataCellStyle="Normal"/>
+    <tableColumn id="9" name="Operating System Architecture Type" totalsRowDxfId="20" dataCellStyle="Normal"/>
+    <tableColumn id="10" name="Number of SQL Instances" totalsRowFunction="custom" totalsRowDxfId="19" dataCellStyle="Normal">
       <totalsRowFormula>SUM(J2:J2)</totalsRowFormula>
     </tableColumn>
+    <tableColumn id="29" name="SQL Services Running" totalsRowDxfId="18"/>
+    <tableColumn id="27" name="SQL Services Stopped" totalsRowDxfId="17"/>
     <tableColumn id="11" name="Number Of Databases" totalsRowFunction="custom" totalsRowDxfId="16" dataCellStyle="Normal">
-      <totalsRowFormula>SUM(K2:K2)</totalsRowFormula>
+      <totalsRowFormula>SUM(M2:M2)</totalsRowFormula>
     </tableColumn>
     <tableColumn id="12" name="Number of Processors" totalsRowFunction="custom" totalsRowDxfId="15" dataCellStyle="Normal">
-      <totalsRowFormula>SUM(L2:L2)</totalsRowFormula>
+      <totalsRowFormula>SUM(N2:N2)</totalsRowFormula>
     </tableColumn>
     <tableColumn id="13" name="Number of Total Cores" totalsRowFunction="custom" totalsRowDxfId="14" dataCellStyle="Normal">
-      <totalsRowFormula>SUM(M2:M2)</totalsRowFormula>
+      <totalsRowFormula>SUM(O2:O2)</totalsRowFormula>
     </tableColumn>
     <tableColumn id="14" name="Number of Logical Processors" totalsRowFunction="custom" totalsRowDxfId="13" dataCellStyle="Normal">
-      <totalsRowFormula>SUM(N2:N2)</totalsRowFormula>
+      <totalsRowFormula>SUM(P2:P2)</totalsRowFormula>
     </tableColumn>
     <tableColumn id="15" name="CPU" totalsRowDxfId="12" dataCellStyle="Normal"/>
     <tableColumn id="16" name="System Memory (MB)" totalsRowDxfId="11" dataCellStyle="Normal"/>
     <tableColumn id="17" name="System Memory (GB)" totalsRowFunction="custom" totalsRowDxfId="10" dataCellStyle="Normal">
-      <totalsRowFormula>SUM(Q2:Q2)</totalsRowFormula>
+      <totalsRowFormula>SUM(S2:S2)</totalsRowFormula>
     </tableColumn>
     <tableColumn id="18" name="Logical Disk Size (GB)" totalsRowFunction="custom" totalsRowDxfId="9" dataCellStyle="Normal">
-      <totalsRowFormula>SUM(R2:R2)</totalsRowFormula>
+      <totalsRowFormula>SUM(T2:T2)</totalsRowFormula>
     </tableColumn>
     <tableColumn id="19" name="Logical Disk Free Space (GB)" totalsRowFunction="custom" totalsRowDxfId="8" dataCellStyle="Normal">
-      <totalsRowFormula>SUM(S2:S2)</totalsRowFormula>
+      <totalsRowFormula>SUM(U2:U2)</totalsRowFormula>
     </tableColumn>
     <tableColumn id="20" name="Logical Disk Size (TB)" totalsRowDxfId="7" dataCellStyle="Normal"/>
     <tableColumn id="21" name="Logical Disk Free Space (TB)" totalsRowDxfId="6" dataCellStyle="Normal"/>
     <tableColumn id="22" name="SuccessPercent" totalsRowDxfId="5" dataCellStyle="Normal"/>
     <tableColumn id="28" name="Kolonne1" totalsRowLabel="Average:" totalsRowDxfId="4" dataCellStyle="Normal"/>
     <tableColumn id="23" name="ProcUtil" totalsRowFunction="custom" totalsRowDxfId="3" dataCellStyle="Normal">
-      <totalsRowFormula>AVERAGE(X2:X2)</totalsRowFormula>
+      <totalsRowFormula>AVERAGE(Z2:Z2)</totalsRowFormula>
     </tableColumn>
     <tableColumn id="24" name="MemoryUtil" totalsRowFunction="custom" totalsRowDxfId="2" dataCellStyle="Normal">
-      <totalsRowFormula>AVERAGE(Y2:Y2)</totalsRowFormula>
+      <totalsRowFormula>AVERAGE(AA2:AA2)</totalsRowFormula>
     </tableColumn>
     <tableColumn id="25" name="NetworkUtil" totalsRowFunction="custom" totalsRowDxfId="1" dataCellStyle="Normal">
-      <totalsRowFormula>AVERAGE(Z2:Z2)</totalsRowFormula>
+      <totalsRowFormula>AVERAGE(AB2:AB2)</totalsRowFormula>
     </tableColumn>
     <tableColumn id="26" name="DiskIOPS" totalsRowFunction="custom" totalsRowDxfId="0" dataCellStyle="Normal">
-      <totalsRowFormula>AVERAGE(AA2:AA2)</totalsRowFormula>
+      <totalsRowFormula>AVERAGE(AC2:AC2)</totalsRowFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -14022,7 +14293,7 @@
   <autoFilter ref="F19:H21"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Calculations"/>
-    <tableColumn id="2" name="Storage GB" dataDxfId="124"/>
+    <tableColumn id="2" name="Storage GB" dataDxfId="128"/>
     <tableColumn id="4" name="Percentage"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -14034,7 +14305,7 @@
   <autoFilter ref="J19:L22"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Calculations"/>
-    <tableColumn id="2" name="Memory GB" dataDxfId="123"/>
+    <tableColumn id="2" name="Memory GB" dataDxfId="127"/>
     <tableColumn id="4" name="Percentage"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -14061,7 +14332,7 @@
     <tableColumn id="8" name="SQL Server Cluster Network Name"/>
     <tableColumn id="9" name="SQL Service State"/>
     <tableColumn id="10" name="SQL Service Start Mode"/>
-    <tableColumn id="11" name="Number Of Databases" dataDxfId="122"/>
+    <tableColumn id="11" name="Number Of Databases" dataDxfId="126"/>
     <tableColumn id="12" name="Current Operating System"/>
     <tableColumn id="13" name="Operating System Service Pack Level"/>
     <tableColumn id="14" name="Operating System Architecture Type"/>
@@ -14078,9 +14349,9 @@
   </sortState>
   <tableColumns count="11">
     <tableColumn id="1" name="Computer Name" dataCellStyle="Normal"/>
-    <tableColumn id="9" name="Machine Type" dataDxfId="121" dataCellStyle="Normal"/>
-    <tableColumn id="10" name="Operated by" dataDxfId="120" dataCellStyle="Normal"/>
-    <tableColumn id="11" name="Environment" dataDxfId="119" dataCellStyle="Normal"/>
+    <tableColumn id="9" name="Machine Type" dataDxfId="125" dataCellStyle="Normal"/>
+    <tableColumn id="10" name="Operated by" dataDxfId="124" dataCellStyle="Normal"/>
+    <tableColumn id="11" name="Environment" dataDxfId="123" dataCellStyle="Normal"/>
     <tableColumn id="2" name="SQL Server Component Name" dataCellStyle="Normal"/>
     <tableColumn id="3" name="Component Version" dataCellStyle="Normal"/>
     <tableColumn id="4" name="Component Service Pack" dataCellStyle="Normal"/>
@@ -14135,18 +14406,18 @@
     <tableColumn id="16" uniqueName="16" name="Number of Processors" totalsRowFunction="custom" queryTableFieldId="16">
       <totalsRowFormula>SUM(H3:H3)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="17" uniqueName="17" name="Number of Cores" totalsRowFunction="custom" queryTableFieldId="17" dataDxfId="118" totalsRowDxfId="62">
+    <tableColumn id="17" uniqueName="17" name="Number of Cores" totalsRowFunction="custom" queryTableFieldId="17" dataDxfId="122" totalsRowDxfId="121">
       <totalsRowFormula>SUM(G3:G3)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="18" uniqueName="18" name="Logical Processor Count" totalsRowFunction="custom" queryTableFieldId="18" dataDxfId="117" totalsRowDxfId="61">
+    <tableColumn id="18" uniqueName="18" name="Logical Processor Count" totalsRowFunction="custom" queryTableFieldId="18" dataDxfId="120" totalsRowDxfId="119">
       <totalsRowFormula>SUM(H3:H3)</totalsRowFormula>
     </tableColumn>
     <tableColumn id="19" uniqueName="19" name="CPU Model" queryTableFieldId="19"/>
-    <tableColumn id="20" uniqueName="20" name="System Memory (MB)" queryTableFieldId="20" dataDxfId="116" totalsRowDxfId="60"/>
-    <tableColumn id="3" uniqueName="3" name="System Memory (GB)" totalsRowFunction="custom" queryTableFieldId="28" dataDxfId="115" totalsRowDxfId="59">
+    <tableColumn id="20" uniqueName="20" name="System Memory (MB)" queryTableFieldId="20" dataDxfId="118" totalsRowDxfId="117"/>
+    <tableColumn id="3" uniqueName="3" name="System Memory (GB)" totalsRowFunction="custom" queryTableFieldId="28" dataDxfId="116" totalsRowDxfId="115">
       <totalsRowFormula>SUM(K3:K3)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="22" uniqueName="22" name="Logical Disk Drive Name" queryTableFieldId="22" dataDxfId="114" totalsRowDxfId="58"/>
+    <tableColumn id="22" uniqueName="22" name="Logical Disk Drive Name" queryTableFieldId="22" dataDxfId="114" totalsRowDxfId="113"/>
     <tableColumn id="4" uniqueName="4" name="Logical Disk Size (GB)" queryTableFieldId="42"/>
     <tableColumn id="5" uniqueName="5" name="Logical Disk Free Space (GB)" queryTableFieldId="41"/>
     <tableColumn id="6" uniqueName="6" name="Total Logical Disk Size (GB)" totalsRowFunction="custom" queryTableFieldId="40">
@@ -14168,15 +14439,15 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabel4" displayName="Tabel4" ref="A1:J2" insertRow="1" totalsRowShown="0" headerRowDxfId="113" headerRowBorderDxfId="112" tableBorderDxfId="111" totalsRowBorderDxfId="110" dataCellStyle="Normal">
-  <autoFilter ref="A1:J2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabel4" displayName="Tabel4" ref="A2:J3" insertRow="1" totalsRowShown="0" headerRowDxfId="112" headerRowBorderDxfId="111" tableBorderDxfId="110" totalsRowBorderDxfId="109" dataCellStyle="Normal">
+  <autoFilter ref="A2:J3"/>
   <tableColumns count="10">
     <tableColumn id="1" name="Computer Name" dataCellStyle="Normal"/>
     <tableColumn id="2" name="Machine Type" dataCellStyle="Normal"/>
     <tableColumn id="3" name="Environment" dataCellStyle="Normal"/>
-    <tableColumn id="4" name="Status" dataDxfId="109" dataCellStyle="Normal"/>
+    <tableColumn id="4" name="Status" dataDxfId="108" dataCellStyle="Normal"/>
     <tableColumn id="6" name="Computer Model" dataCellStyle="Normal"/>
-    <tableColumn id="10" name="CPU Model" dataDxfId="108" dataCellStyle="Normal"/>
+    <tableColumn id="10" name="CPU Model" dataDxfId="107" dataCellStyle="Normal"/>
     <tableColumn id="7" name="Number of Processors" dataCellStyle="Normal"/>
     <tableColumn id="8" name="Number of Cores" dataCellStyle="Normal"/>
     <tableColumn id="9" name="Logical Processor Count" dataCellStyle="Normal"/>
@@ -14198,16 +14469,16 @@
     <tableColumn id="11" name="Operated By"/>
     <tableColumn id="10" name="Environment"/>
     <tableColumn id="12" name="SuccessPercent2"/>
-    <tableColumn id="3" name="ProcUtil" totalsRowFunction="custom" totalsRowDxfId="57" dataCellStyle="Normal">
+    <tableColumn id="3" name="ProcUtil" totalsRowFunction="custom" totalsRowDxfId="106" dataCellStyle="Normal">
       <totalsRowFormula>PERCENTILE(F2:F3, 0.95)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="4" name="MemoryUtil" totalsRowFunction="custom" totalsRowDxfId="56" dataCellStyle="Normal">
+    <tableColumn id="4" name="MemoryUtil" totalsRowFunction="custom" totalsRowDxfId="105" dataCellStyle="Normal">
       <totalsRowFormula>PERCENTILE(G2:G3, 0.95)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="5" name="NetworkUtil" totalsRowFunction="custom" totalsRowDxfId="55" dataCellStyle="Normal">
+    <tableColumn id="5" name="NetworkUtil" totalsRowFunction="custom" totalsRowDxfId="104" dataCellStyle="Normal">
       <totalsRowFormula>PERCENTILE(H2:H3, 0.95)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="6" name="DiskIOPS" totalsRowFunction="custom" totalsRowDxfId="54" dataCellStyle="Normal">
+    <tableColumn id="6" name="DiskIOPS" totalsRowFunction="custom" totalsRowDxfId="103" dataCellStyle="Normal">
       <totalsRowFormula>PERCENTILE(I2:I3, 0.95)</totalsRowFormula>
     </tableColumn>
   </tableColumns>
@@ -15188,10 +15459,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA4"/>
+  <dimension ref="A1:AC4"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+      <selection activeCell="U3" sqref="U3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15205,33 +15476,33 @@
     <col min="7" max="7" width="30.28515625" customWidth="1"/>
     <col min="8" max="8" width="55.140625" customWidth="1"/>
     <col min="9" max="9" width="35.85546875" customWidth="1"/>
-    <col min="10" max="10" width="25.85546875" customWidth="1"/>
-    <col min="11" max="11" width="23" customWidth="1"/>
-    <col min="12" max="12" width="23.140625" customWidth="1"/>
-    <col min="13" max="13" width="23.5703125" customWidth="1"/>
-    <col min="14" max="14" width="29.85546875" customWidth="1"/>
-    <col min="15" max="15" width="50.85546875" customWidth="1"/>
-    <col min="16" max="16" width="23" customWidth="1"/>
-    <col min="17" max="17" width="22.42578125" customWidth="1"/>
-    <col min="18" max="18" width="22.28515625" customWidth="1"/>
-    <col min="19" max="19" width="28.5703125" customWidth="1"/>
-    <col min="20" max="20" width="21.85546875" customWidth="1"/>
-    <col min="21" max="21" width="28.140625" customWidth="1"/>
-    <col min="22" max="22" width="17.140625" customWidth="1"/>
-    <col min="23" max="23" width="17" customWidth="1"/>
-    <col min="24" max="24" width="10.5703125" customWidth="1"/>
-    <col min="25" max="25" width="14.28515625" customWidth="1"/>
-    <col min="26" max="26" width="14.42578125" customWidth="1"/>
-    <col min="27" max="27" width="12" customWidth="1"/>
-    <col min="28" max="28" width="27.5703125" customWidth="1"/>
-    <col min="29" max="29" width="16.7109375" customWidth="1"/>
-    <col min="30" max="30" width="10.140625" customWidth="1"/>
-    <col min="31" max="31" width="13.7109375" customWidth="1"/>
-    <col min="32" max="32" width="14" customWidth="1"/>
-    <col min="33" max="33" width="11" customWidth="1"/>
+    <col min="10" max="12" width="25.85546875" customWidth="1"/>
+    <col min="13" max="13" width="23" customWidth="1"/>
+    <col min="14" max="14" width="23.140625" customWidth="1"/>
+    <col min="15" max="15" width="23.5703125" customWidth="1"/>
+    <col min="16" max="16" width="29.85546875" customWidth="1"/>
+    <col min="17" max="17" width="50.85546875" customWidth="1"/>
+    <col min="18" max="18" width="23" customWidth="1"/>
+    <col min="19" max="19" width="22.42578125" customWidth="1"/>
+    <col min="20" max="20" width="22.28515625" customWidth="1"/>
+    <col min="21" max="21" width="28.5703125" customWidth="1"/>
+    <col min="22" max="22" width="21.85546875" customWidth="1"/>
+    <col min="23" max="23" width="28.140625" customWidth="1"/>
+    <col min="24" max="24" width="17.140625" customWidth="1"/>
+    <col min="25" max="25" width="17" customWidth="1"/>
+    <col min="26" max="26" width="10.5703125" customWidth="1"/>
+    <col min="27" max="27" width="14.28515625" customWidth="1"/>
+    <col min="28" max="28" width="14.42578125" customWidth="1"/>
+    <col min="29" max="29" width="12" customWidth="1"/>
+    <col min="30" max="30" width="27.5703125" customWidth="1"/>
+    <col min="31" max="31" width="16.7109375" customWidth="1"/>
+    <col min="32" max="32" width="10.140625" customWidth="1"/>
+    <col min="33" max="33" width="13.7109375" customWidth="1"/>
+    <col min="34" max="34" width="14" customWidth="1"/>
+    <col min="35" max="35" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -15263,79 +15534,79 @@
         <v>106</v>
       </c>
       <c r="K1" t="s">
+        <v>132</v>
+      </c>
+      <c r="L1" t="s">
+        <v>133</v>
+      </c>
+      <c r="M1" t="s">
         <v>100</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>103</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>104</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>0</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>11</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>90</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>92</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>12</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>107</v>
       </c>
-      <c r="U1" t="s">
+      <c r="W1" t="s">
         <v>108</v>
       </c>
-      <c r="V1" t="s">
+      <c r="X1" t="s">
         <v>105</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Y1" t="s">
         <v>116</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Z1" t="s">
         <v>96</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AA1" t="s">
         <v>97</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AB1" t="s">
         <v>98</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AC1" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A3" s="37"/>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A3" s="38"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
       <c r="J3" s="38">
         <f>SUM(J2:J2)</f>
         <v>0</v>
       </c>
-      <c r="K3" s="38">
-        <f>SUM(K2:K2)</f>
-        <v>0</v>
-      </c>
-      <c r="L3" s="38">
-        <f>SUM(L2:L2)</f>
-        <v>0</v>
-      </c>
+      <c r="K3" s="38"/>
+      <c r="L3" s="38"/>
       <c r="M3" s="38">
         <f>SUM(M2:M2)</f>
         <v>0</v>
@@ -15344,33 +15615,33 @@
         <f>SUM(N2:N2)</f>
         <v>0</v>
       </c>
-      <c r="O3" s="37"/>
-      <c r="P3" s="37"/>
-      <c r="Q3" s="38">
-        <f>SUM(Q2:Q2)</f>
+      <c r="O3" s="38">
+        <f>SUM(O2:O2)</f>
         <v>0</v>
       </c>
-      <c r="R3" s="38">
-        <f>SUM(R2:R2)</f>
+      <c r="P3" s="38">
+        <f>SUM(P2:P2)</f>
         <v>0</v>
       </c>
+      <c r="Q3" s="38"/>
+      <c r="R3" s="38"/>
       <c r="S3" s="38">
         <f>SUM(S2:S2)</f>
         <v>0</v>
       </c>
-      <c r="T3" s="37"/>
-      <c r="U3" s="37"/>
-      <c r="V3" s="37"/>
-      <c r="W3" s="39" t="s">
+      <c r="T3" s="38">
+        <f>SUM(T2:T2)</f>
+        <v>0</v>
+      </c>
+      <c r="U3" s="38">
+        <f>SUM(U2:U2)</f>
+        <v>0</v>
+      </c>
+      <c r="V3" s="38"/>
+      <c r="W3" s="38"/>
+      <c r="X3" s="38"/>
+      <c r="Y3" s="43" t="s">
         <v>117</v>
-      </c>
-      <c r="X3" s="38" t="e">
-        <f>AVERAGE(X2:X2)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Y3" s="38" t="e">
-        <f>AVERAGE(Y2:Y2)</f>
-        <v>#DIV/0!</v>
       </c>
       <c r="Z3" s="38" t="e">
         <f>AVERAGE(Z2:Z2)</f>
@@ -15380,8 +15651,16 @@
         <f>AVERAGE(AA2:AA2)</f>
         <v>#DIV/0!</v>
       </c>
+      <c r="AB3" s="38" t="e">
+        <f>AVERAGE(AB2:AB2)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AC3" s="38" t="e">
+        <f>AVERAGE(AC2:AC2)</f>
+        <v>#DIV/0!</v>
+      </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" s="19"/>
       <c r="B4" s="19"/>
       <c r="C4" s="19"/>
@@ -15404,16 +15683,10 @@
       <c r="T4" s="19"/>
       <c r="U4" s="19"/>
       <c r="V4" s="19"/>
-      <c r="W4" s="20" t="s">
+      <c r="W4" s="19"/>
+      <c r="X4" s="19"/>
+      <c r="Y4" s="20" t="s">
         <v>118</v>
-      </c>
-      <c r="X4" s="36" t="e">
-        <f>PERCENTILE(X2:X2, 0.95)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="Y4" s="36" t="e">
-        <f>PERCENTILE(Y2:Y2, 0.95)</f>
-        <v>#NUM!</v>
       </c>
       <c r="Z4" s="36" t="e">
         <f>PERCENTILE(Z2:Z2, 0.95)</f>
@@ -15423,9 +15696,17 @@
         <f>PERCENTILE(AA2:AA2, 0.95)</f>
         <v>#NUM!</v>
       </c>
+      <c r="AB4" s="36" t="e">
+        <f>PERCENTILE(AB2:AB2, 0.95)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="AC4" s="36" t="e">
+        <f>PERCENTILE(AC2:AC2, 0.95)</f>
+        <v>#NUM!</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="AD1:AD1048576">
+  <conditionalFormatting sqref="AF1:AF1048576">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -15437,7 +15718,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AE1:AE1048576">
+  <conditionalFormatting sqref="AG1:AG1048576">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -15449,7 +15730,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF1:AF1048576">
+  <conditionalFormatting sqref="AH1:AH1048576">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -15461,7 +15742,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AG1:AG1048576">
+  <conditionalFormatting sqref="AI1:AI1048576">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -15473,7 +15754,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="X2">
+  <conditionalFormatting sqref="Z2">
     <cfRule type="colorScale" priority="39">
       <colorScale>
         <cfvo type="min"/>
@@ -15485,7 +15766,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y2">
+  <conditionalFormatting sqref="AA2">
     <cfRule type="colorScale" priority="40">
       <colorScale>
         <cfvo type="min"/>
@@ -15497,7 +15778,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z2">
+  <conditionalFormatting sqref="AB2">
     <cfRule type="colorScale" priority="41">
       <colorScale>
         <cfvo type="min"/>
@@ -15509,7 +15790,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA2">
+  <conditionalFormatting sqref="AC2">
     <cfRule type="colorScale" priority="42">
       <colorScale>
         <cfvo type="min"/>
@@ -16326,7 +16607,7 @@
   <dimension ref="A1:W4"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16485,10 +16766,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16507,49 +16788,65 @@
     <col min="13" max="13" width="23.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="31" t="s">
+    <row r="1" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="41"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
+    </row>
+    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B2" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="C2" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="D1" s="34" t="s">
+      <c r="D2" s="34" t="s">
         <v>131</v>
       </c>
-      <c r="E1" s="32" t="s">
+      <c r="E2" s="32" t="s">
         <v>81</v>
       </c>
-      <c r="F1" s="32" t="s">
+      <c r="F2" s="32" t="s">
         <v>95</v>
       </c>
-      <c r="G1" s="32" t="s">
+      <c r="G2" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="32" t="s">
+      <c r="H2" s="32" t="s">
         <v>88</v>
       </c>
-      <c r="I1" s="33" t="s">
+      <c r="I2" s="33" t="s">
         <v>89</v>
       </c>
-      <c r="J1" s="35" t="s">
+      <c r="J2" s="35" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="5"/>
+    <row r="3" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="5"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:J1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
@@ -17108,10 +17405,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA4"/>
+  <dimension ref="A1:AC4"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1:L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17126,32 +17423,33 @@
     <col min="8" max="8" width="55.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="35.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="50.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="23" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="22.42578125" customWidth="1"/>
-    <col min="18" max="18" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="17" customWidth="1"/>
-    <col min="24" max="24" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="12" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="27.5703125" customWidth="1"/>
-    <col min="29" max="29" width="16.7109375" customWidth="1"/>
-    <col min="30" max="30" width="10.140625" customWidth="1"/>
-    <col min="31" max="31" width="13.7109375" customWidth="1"/>
-    <col min="32" max="32" width="14" customWidth="1"/>
-    <col min="33" max="33" width="11" customWidth="1"/>
+    <col min="11" max="12" width="25.85546875" customWidth="1"/>
+    <col min="13" max="13" width="23" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="50.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="23" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="22.42578125" customWidth="1"/>
+    <col min="20" max="20" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="17" customWidth="1"/>
+    <col min="26" max="26" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="12" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="27.5703125" customWidth="1"/>
+    <col min="31" max="31" width="16.7109375" customWidth="1"/>
+    <col min="32" max="32" width="10.140625" customWidth="1"/>
+    <col min="33" max="33" width="13.7109375" customWidth="1"/>
+    <col min="34" max="34" width="14" customWidth="1"/>
+    <col min="35" max="35" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -17183,58 +17481,64 @@
         <v>106</v>
       </c>
       <c r="K1" t="s">
+        <v>132</v>
+      </c>
+      <c r="L1" t="s">
+        <v>133</v>
+      </c>
+      <c r="M1" t="s">
         <v>100</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>103</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>104</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>0</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>11</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>90</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>92</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>12</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>107</v>
       </c>
-      <c r="U1" t="s">
+      <c r="W1" t="s">
         <v>108</v>
       </c>
-      <c r="V1" t="s">
+      <c r="X1" t="s">
         <v>105</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Y1" t="s">
         <v>116</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Z1" t="s">
         <v>96</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AA1" t="s">
         <v>97</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AB1" t="s">
         <v>98</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AC1" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" s="37"/>
       <c r="B3" s="37"/>
       <c r="C3" s="37"/>
@@ -17248,14 +17552,8 @@
         <f>SUM(J2:J2)</f>
         <v>0</v>
       </c>
-      <c r="K3" s="38">
-        <f>SUM(K2:K2)</f>
-        <v>0</v>
-      </c>
-      <c r="L3" s="38">
-        <f>SUM(L2:L2)</f>
-        <v>0</v>
-      </c>
+      <c r="K3" s="38"/>
+      <c r="L3" s="38"/>
       <c r="M3" s="38">
         <f>SUM(M2:M2)</f>
         <v>0</v>
@@ -17264,33 +17562,33 @@
         <f>SUM(N2:N2)</f>
         <v>0</v>
       </c>
-      <c r="O3" s="37"/>
-      <c r="P3" s="37"/>
-      <c r="Q3" s="38">
-        <f>SUM(Q2:Q2)</f>
+      <c r="O3" s="38">
+        <f>SUM(O2:O2)</f>
         <v>0</v>
       </c>
-      <c r="R3" s="38">
-        <f>SUM(R2:R2)</f>
+      <c r="P3" s="38">
+        <f>SUM(P2:P2)</f>
         <v>0</v>
       </c>
+      <c r="Q3" s="37"/>
+      <c r="R3" s="37"/>
       <c r="S3" s="38">
         <f>SUM(S2:S2)</f>
         <v>0</v>
       </c>
-      <c r="T3" s="37"/>
-      <c r="U3" s="37"/>
+      <c r="T3" s="38">
+        <f>SUM(T2:T2)</f>
+        <v>0</v>
+      </c>
+      <c r="U3" s="38">
+        <f>SUM(U2:U2)</f>
+        <v>0</v>
+      </c>
       <c r="V3" s="37"/>
-      <c r="W3" s="39" t="s">
+      <c r="W3" s="37"/>
+      <c r="X3" s="37"/>
+      <c r="Y3" s="39" t="s">
         <v>117</v>
-      </c>
-      <c r="X3" s="38" t="e">
-        <f>AVERAGE(X2:X2)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Y3" s="38" t="e">
-        <f>AVERAGE(Y2:Y2)</f>
-        <v>#DIV/0!</v>
       </c>
       <c r="Z3" s="38" t="e">
         <f>AVERAGE(Z2:Z2)</f>
@@ -17300,8 +17598,16 @@
         <f>AVERAGE(AA2:AA2)</f>
         <v>#DIV/0!</v>
       </c>
+      <c r="AB3" s="38" t="e">
+        <f>AVERAGE(AB2:AB2)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AC3" s="38" t="e">
+        <f>AVERAGE(AC2:AC2)</f>
+        <v>#DIV/0!</v>
+      </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" s="19"/>
       <c r="B4" s="19"/>
       <c r="C4" s="19"/>
@@ -17324,16 +17630,10 @@
       <c r="T4" s="19"/>
       <c r="U4" s="19"/>
       <c r="V4" s="19"/>
-      <c r="W4" s="20" t="s">
+      <c r="W4" s="19"/>
+      <c r="X4" s="19"/>
+      <c r="Y4" s="20" t="s">
         <v>118</v>
-      </c>
-      <c r="X4" s="36" t="e">
-        <f>PERCENTILE(X2:X2, 0.95)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="Y4" s="36" t="e">
-        <f>PERCENTILE(Y2:Y2, 0.95)</f>
-        <v>#NUM!</v>
       </c>
       <c r="Z4" s="36" t="e">
         <f>PERCENTILE(Z2:Z2, 0.95)</f>
@@ -17343,9 +17643,17 @@
         <f>PERCENTILE(AA2:AA2, 0.95)</f>
         <v>#NUM!</v>
       </c>
+      <c r="AB4" s="36" t="e">
+        <f>PERCENTILE(AB2:AB2, 0.95)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="AC4" s="36" t="e">
+        <f>PERCENTILE(AC2:AC2, 0.95)</f>
+        <v>#NUM!</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="AD1:AD1048576">
+  <conditionalFormatting sqref="AF1:AF1048576">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
@@ -17357,7 +17665,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AE1:AE1048576">
+  <conditionalFormatting sqref="AG1:AG1048576">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
@@ -17369,7 +17677,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF1:AF1048576">
+  <conditionalFormatting sqref="AH1:AH1048576">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -17381,7 +17689,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AG1:AG1048576">
+  <conditionalFormatting sqref="AI1:AI1048576">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -17393,7 +17701,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="X2">
+  <conditionalFormatting sqref="Z2">
     <cfRule type="colorScale" priority="31">
       <colorScale>
         <cfvo type="min"/>
@@ -17405,7 +17713,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y2">
+  <conditionalFormatting sqref="AA2">
     <cfRule type="colorScale" priority="32">
       <colorScale>
         <cfvo type="min"/>
@@ -17417,7 +17725,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z2">
+  <conditionalFormatting sqref="AB2">
     <cfRule type="colorScale" priority="33">
       <colorScale>
         <cfvo type="min"/>
@@ -17429,7 +17737,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA2">
+  <conditionalFormatting sqref="AC2">
     <cfRule type="colorScale" priority="34">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>